<commit_message>
Update template w/ terminology bindings
</commit_message>
<xml_diff>
--- a/exporterat/akutmall_undervisningsexempel_2a.xlsx
+++ b/exporterat/akutmall_undervisningsexempel_2a.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="396">
   <si>
     <t/>
   </si>
@@ -111,36 +111,36 @@
     <t>ARCHETYPE / EVALUATION</t>
   </si>
   <si>
+    <t>Clear delineation between the scope of a problem versus a diagnosis is not easy to achieve in practice. For the purposes of clinical documentation with this archetype, problem and diagnosis are regarded as a continuum, with increasing levels of detail and supportive evidence usually providing weight towards the label of 'diagnosis'.</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-EVALUATION.problem_diagnosis.v1, 'Problem/Diagnosis']</t>
+  </si>
+  <si>
+    <t>Problem/Diagnosis name</t>
+  </si>
+  <si>
+    <t>Identification of the problem or diagnosis, by name.</t>
+  </si>
+  <si>
+    <t>TEXT</t>
+  </si>
+  <si>
+    <t>Coding of the name of the problem or diagnosis with a terminology is preferred, where possible.</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-EVALUATION.problem_diagnosis.v1, 'Problem/Diagnosis']/data[at0001]/items[at0002]</t>
+  </si>
+  <si>
+    <t>Clinical description</t>
+  </si>
+  <si>
+    <t>Narrative description about the problem or diagnosis.</t>
+  </si>
+  <si>
     <t>Optional</t>
   </si>
   <si>
-    <t>Clear delineation between the scope of a problem versus a diagnosis is not easy to achieve in practice. For the purposes of clinical documentation with this archetype, problem and diagnosis are regarded as a continuum, with increasing levels of detail and supportive evidence usually providing weight towards the label of 'diagnosis'.</t>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-EVALUATION.problem_diagnosis.v1, 'Problem/Diagnosis']</t>
-  </si>
-  <si>
-    <t>Problem/Diagnosis name</t>
-  </si>
-  <si>
-    <t>Identification of the problem or diagnosis, by name.</t>
-  </si>
-  <si>
-    <t>TEXT</t>
-  </si>
-  <si>
-    <t>Coding of the name of the problem or diagnosis with a terminology is preferred, where possible.</t>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-EVALUATION.problem_diagnosis.v1, 'Problem/Diagnosis']/data[at0001]/items[at0002]</t>
-  </si>
-  <si>
-    <t>Clinical description</t>
-  </si>
-  <si>
-    <t>Narrative description about the problem or diagnosis.</t>
-  </si>
-  <si>
     <t>Use to provide background and context, including evolution, episodes or exacerbations, progress and any other relevant details, about the problem or diagnosis.</t>
   </si>
   <si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>Identification of a simple body site for the location of the problem or diagnosis.</t>
+  </si>
+  <si>
+    <t>CODED TEXT</t>
   </si>
   <si>
     <t xml:space="preserve">Coding of the name of the anatomical location with a terminology is preferred, where possible.
@@ -1506,24 +1509,24 @@
         <v>16</v>
       </c>
       <c r="H4" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="I4" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="I4" t="s" s="0">
+      <c r="J4" t="s" s="0">
         <v>32</v>
-      </c>
-      <c r="J4" t="s" s="0">
-        <v>33</v>
       </c>
     </row>
     <row r="5">
       <c r="D5" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="F5" t="s" s="0">
         <v>35</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>36</v>
       </c>
       <c r="G5" t="s" s="0">
         <v>16</v>
@@ -1532,27 +1535,27 @@
         <v>17</v>
       </c>
       <c r="I5" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="J5" t="s" s="0">
         <v>37</v>
-      </c>
-      <c r="J5" t="s" s="0">
-        <v>38</v>
       </c>
     </row>
     <row r="6">
       <c r="D6" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="E6" t="s" s="0">
-        <v>40</v>
-      </c>
       <c r="F6" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G6" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I6" t="s" s="0">
         <v>41</v>
@@ -1569,7 +1572,7 @@
         <v>44</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="G7" t="s" s="0">
         <v>16</v>
@@ -1578,18 +1581,18 @@
         <v>23</v>
       </c>
       <c r="I7" t="s" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J7" t="s" s="0">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8">
       <c r="D8" t="s" s="0">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F8" t="s" s="0">
         <v>21</v>
@@ -1601,87 +1604,87 @@
         <v>23</v>
       </c>
       <c r="I8" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J8" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9">
       <c r="D9" t="s" s="0">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G9" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H9" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I9" t="s" s="0">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J9" t="s" s="0">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10">
       <c r="D10" t="s" s="0">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G10" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H10" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I10" t="s" s="0">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J10" t="s" s="0">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11">
       <c r="D11" t="s" s="0">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F11" t="s" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G11" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H11" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I11" t="s" s="0">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J11" t="s" s="0">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12">
       <c r="D12" t="s" s="0">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E12" t="s" s="0">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F12" t="s" s="0">
         <v>21</v>
@@ -1693,61 +1696,61 @@
         <v>23</v>
       </c>
       <c r="I12" t="s" s="0">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J12" t="s" s="0">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13">
       <c r="D13" t="s" s="0">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E13" t="s" s="0">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F13" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G13" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H13" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J13" t="s" s="0">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14">
       <c r="D14" t="s" s="0">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E14" t="s" s="0">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F14" t="s" s="0">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G14" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H14" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I14" t="s" s="0">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J14" t="s" s="0">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15">
       <c r="D15" t="s" s="0">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E15" t="s" s="0">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F15" t="s" s="0">
         <v>21</v>
@@ -1759,70 +1762,70 @@
         <v>23</v>
       </c>
       <c r="I15" t="s" s="0">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J15" t="s" s="0">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16">
       <c r="D16" t="s" s="0">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E16" t="s" s="0">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F16" t="s" s="0">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G16" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H16" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J16" t="s" s="0">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17">
       <c r="D17" t="s" s="0">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E17" t="s" s="0">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F17" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G17" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H17" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J17" t="s" s="0">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18">
       <c r="D18" t="s" s="0">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E18" t="s" s="0">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F18" t="s" s="0">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G18" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H18" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J18" t="s" s="0">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19">
@@ -1830,7 +1833,7 @@
         <v>19</v>
       </c>
       <c r="E19" t="s" s="0">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F19" t="s" s="0">
         <v>21</v>
@@ -1842,47 +1845,47 @@
         <v>23</v>
       </c>
       <c r="I19" t="s" s="0">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J19" t="s" s="0">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s" s="0">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D20" t="s" s="0">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E20" t="s" s="0">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F20" t="s" s="0">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G20" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H20" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J20" t="s" s="0">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21">
       <c r="D21" t="s" s="0">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E21" t="s" s="0">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F21" t="s" s="0">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="G21" t="s" s="0">
         <v>16</v>
@@ -1891,102 +1894,102 @@
         <v>17</v>
       </c>
       <c r="I21" t="s" s="0">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J21" t="s" s="0">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22">
       <c r="D22" t="s" s="0">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E22" t="s" s="0">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F22" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G22" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H22" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I22" t="s" s="0">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J22" t="s" s="0">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23">
       <c r="D23" t="s" s="0">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E23" t="s" s="0">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F23" t="s" s="0">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G23" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H23" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I23" t="s" s="0">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J23" t="s" s="0">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24">
       <c r="D24" t="s" s="0">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E24" t="s" s="0">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F24" t="s" s="0">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G24" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H24" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I24" t="s" s="0">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J24" t="s" s="0">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25">
       <c r="D25" t="s" s="0">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E25" t="s" s="0">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F25" t="s" s="0">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G25" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H25" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I25" t="s" s="0">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J25" t="s" s="0">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26">
@@ -1994,30 +1997,30 @@
         <v>5</v>
       </c>
       <c r="E26" t="s" s="0">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F26" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G26" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H26" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I26" t="s" s="0">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J26" t="s" s="0">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27">
       <c r="D27" t="s" s="0">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E27" t="s" s="0">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F27" t="s" s="0">
         <v>21</v>
@@ -2029,18 +2032,18 @@
         <v>23</v>
       </c>
       <c r="I27" t="s" s="0">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J27" t="s" s="0">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28">
       <c r="D28" t="s" s="0">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E28" t="s" s="0">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F28" t="s" s="0">
         <v>21</v>
@@ -2052,150 +2055,150 @@
         <v>23</v>
       </c>
       <c r="J28" t="s" s="0">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s" s="0">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C29" t="s" s="0">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D29" t="s" s="0">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E29" t="s" s="0">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F29" t="s" s="0">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G29" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H29" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J29" t="s" s="0">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s" s="0">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C30" t="s" s="0">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D30" t="s" s="0">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E30" t="s" s="0">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F30" t="s" s="0">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G30" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H30" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J30" t="s" s="0">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="31">
       <c r="D31" t="s" s="0">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E31" t="s" s="0">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F31" t="s" s="0">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G31" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H31" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I31" t="s" s="0">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J31" t="s" s="0">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32">
       <c r="D32" t="s" s="0">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E32" t="s" s="0">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F32" t="s" s="0">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G32" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H32" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J32" t="s" s="0">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33">
       <c r="D33" t="s" s="0">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E33" t="s" s="0">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F33" t="s" s="0">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G33" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H33" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J33" t="s" s="0">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34">
       <c r="D34" t="s" s="0">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E34" t="s" s="0">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F34" t="s" s="0">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G34" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H34" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J34" t="s" s="0">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35">
       <c r="D35" t="s" s="0">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E35" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F35" t="s" s="0">
         <v>21</v>
@@ -2207,15 +2210,15 @@
         <v>23</v>
       </c>
       <c r="J35" t="s" s="0">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36">
       <c r="D36" t="s" s="0">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E36" t="s" s="0">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F36" t="s" s="0">
         <v>21</v>
@@ -2227,58 +2230,58 @@
         <v>23</v>
       </c>
       <c r="J36" t="s" s="0">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37">
       <c r="D37" t="s" s="0">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E37" t="s" s="0">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F37" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G37" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H37" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I37" t="s" s="0">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="J37" t="s" s="0">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38">
       <c r="D38" t="s" s="0">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E38" t="s" s="0">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F38" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G38" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H38" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J38" t="s" s="0">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="39">
       <c r="D39" t="s" s="0">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E39" t="s" s="0">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F39" t="s" s="0">
         <v>21</v>
@@ -2287,18 +2290,18 @@
         <v>22</v>
       </c>
       <c r="H39" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J39" t="s" s="0">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="40">
       <c r="D40" t="s" s="0">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E40" t="s" s="0">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F40" t="s" s="0">
         <v>21</v>
@@ -2307,87 +2310,87 @@
         <v>16</v>
       </c>
       <c r="H40" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I40" t="s" s="0">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="J40" t="s" s="0">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="41">
       <c r="D41" t="s" s="0">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E41" t="s" s="0">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F41" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G41" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H41" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I41" t="s" s="0">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="J41" t="s" s="0">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="42">
       <c r="D42" t="s" s="0">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E42" t="s" s="0">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F42" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G42" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H42" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I42" t="s" s="0">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J42" t="s" s="0">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="43">
       <c r="D43" t="s" s="0">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E43" t="s" s="0">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F43" t="s" s="0">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G43" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H43" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J43" t="s" s="0">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="44">
       <c r="D44" t="s" s="0">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E44" t="s" s="0">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F44" t="s" s="0">
         <v>21</v>
@@ -2396,10 +2399,10 @@
         <v>22</v>
       </c>
       <c r="H44" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J44" t="s" s="0">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="45">
@@ -2419,159 +2422,159 @@
         <v>23</v>
       </c>
       <c r="I45" t="s" s="0">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="J45" t="s" s="0">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" t="s" s="0">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C46" t="s" s="0">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D46" t="s" s="0">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E46" t="s" s="0">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F46" t="s" s="0">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G46" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H46" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J46" t="s" s="0">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="47">
       <c r="D47" t="s" s="0">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E47" t="s" s="0">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F47" t="s" s="0">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G47" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H47" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I47" t="s" s="0">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="J47" t="s" s="0">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="48">
       <c r="D48" t="s" s="0">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E48" t="s" s="0">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F48" t="s" s="0">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G48" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H48" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I48" t="s" s="0">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="J48" t="s" s="0">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="49">
       <c r="D49" t="s" s="0">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E49" t="s" s="0">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F49" t="s" s="0">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G49" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H49" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I49" t="s" s="0">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="J49" t="s" s="0">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="50">
       <c r="D50" t="s" s="0">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E50" t="s" s="0">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F50" t="s" s="0">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G50" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H50" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I50" t="s" s="0">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="J50" t="s" s="0">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="51">
       <c r="D51" t="s" s="0">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E51" t="s" s="0">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F51" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G51" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H51" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I51" t="s" s="0">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="J51" t="s" s="0">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="52">
       <c r="D52" t="s" s="0">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E52" t="s" s="0">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F52" t="s" s="0">
         <v>21</v>
@@ -2583,153 +2586,153 @@
         <v>23</v>
       </c>
       <c r="I52" t="s" s="0">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="J52" t="s" s="0">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="s" s="0">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C53" t="s" s="0">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D53" t="s" s="0">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E53" t="s" s="0">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F53" t="s" s="0">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G53" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H53" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J53" t="s" s="0">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="54">
       <c r="D54" t="s" s="0">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E54" t="s" s="0">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="F54" t="s" s="0">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="G54" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H54" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I54" t="s" s="0">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="J54" t="s" s="0">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="55">
       <c r="D55" t="s" s="0">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E55" t="s" s="0">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="F55" t="s" s="0">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G55" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H55" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J55" t="s" s="0">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="56">
       <c r="D56" t="s" s="0">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E56" t="s" s="0">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F56" t="s" s="0">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="G56" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H56" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J56" t="s" s="0">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="57">
       <c r="D57" t="s" s="0">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E57" t="s" s="0">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F57" t="s" s="0">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="G57" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H57" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J57" t="s" s="0">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="58">
       <c r="D58" t="s" s="0">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E58" t="s" s="0">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F58" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G58" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H58" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I58" t="s" s="0">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="J58" t="s" s="0">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="59">
       <c r="D59" t="s" s="0">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E59" t="s" s="0">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="F59" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G59" t="s" s="0">
         <v>16</v>
@@ -2738,81 +2741,81 @@
         <v>23</v>
       </c>
       <c r="I59" t="s" s="0">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="J59" t="s" s="0">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="60">
       <c r="D60" t="s" s="0">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E60" t="s" s="0">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F60" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G60" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H60" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J60" t="s" s="0">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="61">
       <c r="D61" t="s" s="0">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E61" t="s" s="0">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F61" t="s" s="0">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G61" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H61" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J61" t="s" s="0">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="62">
       <c r="D62" t="s" s="0">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E62" t="s" s="0">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F62" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G62" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H62" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I62" t="s" s="0">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="J62" t="s" s="0">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="63">
       <c r="D63" t="s" s="0">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E63" t="s" s="0">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F63" t="s" s="0">
         <v>21</v>
@@ -2821,21 +2824,21 @@
         <v>16</v>
       </c>
       <c r="H63" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I63" t="s" s="0">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="J63" t="s" s="0">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="64">
       <c r="D64" t="s" s="0">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E64" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F64" t="s" s="0">
         <v>21</v>
@@ -2844,13 +2847,13 @@
         <v>22</v>
       </c>
       <c r="H64" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I64" t="s" s="0">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="J64" t="s" s="0">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="65">
@@ -2870,159 +2873,159 @@
         <v>23</v>
       </c>
       <c r="I65" t="s" s="0">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J65" t="s" s="0">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="66">
       <c r="B66" t="s" s="0">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C66" t="s" s="0">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D66" t="s" s="0">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E66" t="s" s="0">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F66" t="s" s="0">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G66" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H66" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J66" t="s" s="0">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="67">
       <c r="D67" t="s" s="0">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E67" t="s" s="0">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F67" t="s" s="0">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G67" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H67" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I67" t="s" s="0">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="J67" t="s" s="0">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="68">
       <c r="D68" t="s" s="0">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E68" t="s" s="0">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F68" t="s" s="0">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G68" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H68" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I68" t="s" s="0">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="J68" t="s" s="0">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="69">
       <c r="D69" t="s" s="0">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E69" t="s" s="0">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F69" t="s" s="0">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G69" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H69" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I69" t="s" s="0">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="J69" t="s" s="0">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="70">
       <c r="D70" t="s" s="0">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E70" t="s" s="0">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F70" t="s" s="0">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G70" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H70" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I70" t="s" s="0">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="J70" t="s" s="0">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="71">
       <c r="D71" t="s" s="0">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E71" t="s" s="0">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F71" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G71" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H71" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I71" t="s" s="0">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="J71" t="s" s="0">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="72">
       <c r="D72" t="s" s="0">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E72" t="s" s="0">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F72" t="s" s="0">
         <v>21</v>
@@ -3034,259 +3037,259 @@
         <v>23</v>
       </c>
       <c r="I72" t="s" s="0">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="J72" t="s" s="0">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="73">
       <c r="B73" t="s" s="0">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C73" t="s" s="0">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D73" t="s" s="0">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E73" t="s" s="0">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F73" t="s" s="0">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G73" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H73" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J73" t="s" s="0">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="74">
       <c r="D74" t="s" s="0">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E74" t="s" s="0">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="F74" t="s" s="0">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G74" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H74" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I74" t="s" s="0">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="J74" t="s" s="0">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="75">
       <c r="D75" t="s" s="0">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E75" t="s" s="0">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="F75" t="s" s="0">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G75" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H75" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J75" t="s" s="0">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="76">
       <c r="D76" t="s" s="0">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E76" t="s" s="0">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F76" t="s" s="0">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="G76" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H76" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J76" t="s" s="0">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="77">
       <c r="D77" t="s" s="0">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E77" t="s" s="0">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F77" t="s" s="0">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="G77" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H77" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I77" t="s" s="0">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="J77" t="s" s="0">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="78">
       <c r="D78" t="s" s="0">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E78" t="s" s="0">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="F78" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G78" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H78" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I78" t="s" s="0">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="J78" t="s" s="0">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="79">
       <c r="D79" t="s" s="0">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E79" t="s" s="0">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="F79" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G79" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H79" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J79" t="s" s="0">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="80">
       <c r="D80" t="s" s="0">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E80" t="s" s="0">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F80" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G80" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H80" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I80" t="s" s="0">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="J80" t="s" s="0">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="81">
       <c r="D81" t="s" s="0">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E81" t="s" s="0">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F81" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G81" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H81" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J81" t="s" s="0">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="82">
       <c r="D82" t="s" s="0">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E82" t="s" s="0">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F82" t="s" s="0">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="G82" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H82" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J82" t="s" s="0">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="83">
       <c r="D83" t="s" s="0">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E83" t="s" s="0">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="F83" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G83" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H83" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I83" t="s" s="0">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="J83" t="s" s="0">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="84">
       <c r="D84" t="s" s="0">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E84" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F84" t="s" s="0">
         <v>21</v>
@@ -3298,104 +3301,104 @@
         <v>23</v>
       </c>
       <c r="J84" t="s" s="0">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="85">
       <c r="D85" t="s" s="0">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E85" t="s" s="0">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="F85" t="s" s="0">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G85" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H85" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I85" t="s" s="0">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="J85" t="s" s="0">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="86">
       <c r="D86" t="s" s="0">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E86" t="s" s="0">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="F86" t="s" s="0">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G86" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H86" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J86" t="s" s="0">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="87">
       <c r="D87" t="s" s="0">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E87" t="s" s="0">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F87" t="s" s="0">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="G87" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H87" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J87" t="s" s="0">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="88">
       <c r="D88" t="s" s="0">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E88" t="s" s="0">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F88" t="s" s="0">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="G88" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H88" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I88" t="s" s="0">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="J88" t="s" s="0">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="89">
       <c r="D89" t="s" s="0">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E89" t="s" s="0">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="F89" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G89" t="s" s="0">
         <v>22</v>
@@ -3404,41 +3407,41 @@
         <v>23</v>
       </c>
       <c r="I89" t="s" s="0">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="J89" t="s" s="0">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="90">
       <c r="D90" t="s" s="0">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E90" t="s" s="0">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="F90" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G90" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H90" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J90" t="s" s="0">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="91">
       <c r="D91" t="s" s="0">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E91" t="s" s="0">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F91" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G91" t="s" s="0">
         <v>22</v>
@@ -3447,61 +3450,61 @@
         <v>23</v>
       </c>
       <c r="I91" t="s" s="0">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="J91" t="s" s="0">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="92">
       <c r="D92" t="s" s="0">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E92" t="s" s="0">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F92" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G92" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H92" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J92" t="s" s="0">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="93">
       <c r="D93" t="s" s="0">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E93" t="s" s="0">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F93" t="s" s="0">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="G93" t="s" s="0">
         <v>22</v>
       </c>
       <c r="H93" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J93" t="s" s="0">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="94">
       <c r="D94" t="s" s="0">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E94" t="s" s="0">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="F94" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G94" t="s" s="0">
         <v>22</v>
@@ -3510,18 +3513,18 @@
         <v>23</v>
       </c>
       <c r="I94" t="s" s="0">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="J94" t="s" s="0">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="95">
       <c r="D95" t="s" s="0">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E95" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F95" t="s" s="0">
         <v>21</v>
@@ -3533,30 +3536,30 @@
         <v>23</v>
       </c>
       <c r="J95" t="s" s="0">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="96">
       <c r="D96" t="s" s="0">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E96" t="s" s="0">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F96" t="s" s="0">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="G96" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H96" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I96" t="s" s="0">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="J96" t="s" s="0">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="97">
@@ -3564,27 +3567,27 @@
         <v>43</v>
       </c>
       <c r="E97" t="s" s="0">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="F97" t="s" s="0">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="G97" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H97" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J97" t="s" s="0">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="98">
       <c r="D98" t="s" s="0">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="E98" t="s" s="0">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F98" t="s" s="0">
         <v>21</v>
@@ -3593,10 +3596,10 @@
         <v>22</v>
       </c>
       <c r="H98" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J98" t="s" s="0">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="99">
@@ -3604,7 +3607,7 @@
         <v>19</v>
       </c>
       <c r="E99" t="s" s="0">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F99" t="s" s="0">
         <v>21</v>
@@ -3616,274 +3619,274 @@
         <v>23</v>
       </c>
       <c r="I99" t="s" s="0">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J99" t="s" s="0">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="100">
       <c r="B100" t="s" s="0">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C100" t="s" s="0">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D100" t="s" s="0">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E100" t="s" s="0">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F100" t="s" s="0">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G100" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H100" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J100" t="s" s="0">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="101">
       <c r="B101" t="s" s="0">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C101" t="s" s="0">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D101" t="s" s="0">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="E101" t="s" s="0">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="F101" t="s" s="0">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G101" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H101" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I101" t="s" s="0">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="J101" t="s" s="0">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="102">
       <c r="D102" t="s" s="0">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="E102" t="s" s="0">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="F102" t="s" s="0">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="G102" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H102" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J102" t="s" s="0">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="103">
       <c r="D103" t="s" s="0">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="E103" t="s" s="0">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="F103" t="s" s="0">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="G103" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H103" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I103" t="s" s="0">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="J103" t="s" s="0">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="104">
       <c r="D104" t="s" s="0">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="E104" t="s" s="0">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="F104" t="s" s="0">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="G104" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H104" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I104" t="s" s="0">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="J104" t="s" s="0">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="105">
       <c r="D105" t="s" s="0">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="E105" t="s" s="0">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="F105" t="s" s="0">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="G105" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H105" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J105" t="s" s="0">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="106">
       <c r="D106" t="s" s="0">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="E106" t="s" s="0">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="F106" t="s" s="0">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="G106" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H106" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J106" t="s" s="0">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="107">
       <c r="D107" t="s" s="0">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="E107" t="s" s="0">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="F107" t="s" s="0">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="G107" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H107" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J107" t="s" s="0">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="108">
       <c r="D108" t="s" s="0">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="E108" t="s" s="0">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="F108" t="s" s="0">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="G108" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H108" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J108" t="s" s="0">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="109">
       <c r="D109" t="s" s="0">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="E109" t="s" s="0">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="F109" t="s" s="0">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="G109" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H109" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J109" t="s" s="0">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="110">
       <c r="D110" t="s" s="0">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E110" t="s" s="0">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="F110" t="s" s="0">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="G110" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H110" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I110" t="s" s="0">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="J110" t="s" s="0">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="111">
       <c r="D111" t="s" s="0">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="E111" t="s" s="0">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="F111" t="s" s="0">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="G111" t="s" s="0">
         <v>16</v>
       </c>
       <c r="H111" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J111" t="s" s="0">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="112">
@@ -3891,7 +3894,7 @@
         <v>19</v>
       </c>
       <c r="E112" t="s" s="0">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="F112" t="s" s="0">
         <v>21</v>
@@ -3903,10 +3906,10 @@
         <v>23</v>
       </c>
       <c r="I112" t="s" s="0">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="J112" t="s" s="0">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
   </sheetData>

</xml_diff>